<commit_message>
Fix for broken Tests automatically generated from Katalon
</commit_message>
<xml_diff>
--- a/TestFiles/File for Dummy MPN.xlsx
+++ b/TestFiles/File for Dummy MPN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PIR_Details\GBS\Alternate Finder\Latest Format Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gssprpra\git\KatalonStudioCodeRep1\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC8E5AC-CAD1-4F1A-8AE0-888DF0B6BA94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698741BB-612B-4C19-B720-C72E1C265AD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     </r>
   </si>
   <si>
-    <t>gsstjaya</t>
-  </si>
-  <si>
     <t>NORNTUM8901RL02</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>PIR-TEST-0005</t>
+  </si>
+  <si>
+    <t>gssprpra</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,44 +576,44 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -624,12 +624,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BA3138D820A29840B950BA4CF954B452" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac9e6ede99833e51c68e6b5545a04474">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aae12c555ce7ed9979d5a752b5dc44a8">
     <xsd:element name="properties">
@@ -743,6 +737,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -753,21 +753,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99FAE743-A39A-421F-B5B3-CCC1CCC21FF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A12EF8C-AF2D-421D-8475-3F46CAC99828}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -783,6 +768,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99FAE743-A39A-421F-B5B3-CCC1CCC21FF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB89A8FF-89EF-4A24-8404-6CFEDB39E983}">
   <ds:schemaRefs>

</xml_diff>